<commit_message>
test queries for game.  Update effort logs book
</commit_message>
<xml_diff>
--- a/docs/efforts/Dustin Bramos.xlsx
+++ b/docs/efforts/Dustin Bramos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9AD9B4-B6FD-4E1F-9D46-38339D954746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D6E3AC-A1C3-4EFA-9385-62DDEDC86A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>6[CS, IT], 5</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 5, 6[CS]</t>
+  </si>
+  <si>
+    <t>Created the History page's query and helped with controllers. Created a MySQL script to completely fill the database with test data. Made a small change to the ERD. Collaborated on the powerpoint presentation.</t>
+  </si>
+  <si>
+    <t>userQueries.php, userControllers.php, Sprint4.pptx, Test Data Insertion Script.sql and GPTMS_ERD.mwb</t>
+  </si>
+  <si>
+    <t>The query inside userQueries.php, the script inside the test insertion script, the Sprint 4 powerpoint, and the database ERD.</t>
   </si>
 </sst>
 </file>
@@ -314,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,6 +357,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -355,24 +388,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -686,38 +701,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
@@ -738,10 +753,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="8">
         <v>16</v>
       </c>
@@ -762,10 +777,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="10">
         <v>20</v>
       </c>
@@ -786,10 +801,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="11">
         <v>22</v>
       </c>
@@ -809,23 +824,35 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12">
+        <v>35</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="9"/>
@@ -834,10 +861,10 @@
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="9"/>
@@ -846,10 +873,10 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="9"/>
@@ -858,10 +885,10 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="9"/>
@@ -870,10 +897,10 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="9"/>
@@ -882,10 +909,10 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
@@ -894,10 +921,10 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="9"/>
@@ -906,10 +933,10 @@
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
@@ -919,6 +946,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -932,11 +964,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -946,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -960,47 +987,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1126,22 +1153,22 @@
         <v>27</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
update database with hints for each hole
</commit_message>
<xml_diff>
--- a/docs/efforts/Dustin Bramos.xlsx
+++ b/docs/efforts/Dustin Bramos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEA6CE1-F761-4F9A-95C5-57012FFCB8BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF70E319-6A37-4629-B4CE-2992D6DDAFE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,6 +372,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -382,24 +403,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -713,38 +716,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
@@ -765,10 +768,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="8">
         <v>16</v>
       </c>
@@ -789,10 +792,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="10">
         <v>20</v>
       </c>
@@ -812,11 +815,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="11">
         <v>22</v>
       </c>
@@ -836,11 +839,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="12">
         <v>35</v>
       </c>
@@ -861,10 +864,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="11">
         <v>36</v>
       </c>
@@ -885,22 +888,26 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="14">
+        <v>32</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="9"/>
@@ -909,10 +916,10 @@
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="9"/>
@@ -921,10 +928,10 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="9"/>
@@ -933,10 +940,10 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
@@ -945,10 +952,10 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="9"/>
@@ -957,10 +964,10 @@
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
@@ -970,6 +977,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -983,11 +995,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -997,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1011,47 +1018,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">

</xml_diff>